<commit_message>
ENH: Add super minimal microphone feature demo
</commit_message>
<xml_diff>
--- a/psychopy/demos/builder/Feature Demos/microphone/phrases.xlsx
+++ b/psychopy/demos/builder/Feature Demos/microphone/phrases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\My Drive\My Pavlovia Demos\pronunciationChecker\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\GitHub\psychopy\psychopy\demos\builder\Feature Demos\microphone\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39B146C4-0AEB-4F01-A0B0-3711457F46E1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CECF04-CAEA-4BE1-8BAB-A21933B2E94D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,39 +96,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
-    <t>C’est simple comme bonjour </t>
+    <t>phrase</t>
   </si>
   <si>
-    <t>On n’est pas sorti de l’auberge</t>
+    <t>She sells sea shells by the sea shore</t>
   </si>
   <si>
-    <t>Être dans la galère</t>
+    <t>Peter Piper picked a peck of pickled peppers</t>
   </si>
   <si>
-    <t>Mettre les points sur les i</t>
+    <t>How much wood would a wood chuck chuck if a wood chuck could chuck wood?</t>
   </si>
   <si>
-    <t>À qui mieux mieux</t>
+    <t>How can a clam cram into a clean cream can?</t>
   </si>
   <si>
-    <t>Il ne faut pas pousser mémé dans les orties</t>
-  </si>
-  <si>
-    <t>Ça ne casse pas trois pattes à un canard</t>
-  </si>
-  <si>
-    <t>Pisser dans un violon</t>
-  </si>
-  <si>
-    <t>Chacun voit midi à sa porte</t>
-  </si>
-  <si>
-    <t>Au petit bonheur la chance</t>
-  </si>
-  <si>
-    <t>phrase</t>
+    <t>I saw Susie sitting in a shoeshine shop</t>
   </si>
 </sst>
 </file>
@@ -523,11 +508,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.7109375" defaultRowHeight="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -538,57 +523,32 @@
   <sheetData>
     <row r="1" spans="1:1" s="2" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>